<commit_message>
update: add tools to test paper C
</commit_message>
<xml_diff>
--- a/tester/tools/test_C/leaderboard.xlsx
+++ b/tester/tools/test_C/leaderboard.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,28 +511,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>王章宇</t>
+          <t>庄伟超</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BUAATRANS2023</t>
+          <t>异乡人</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1982777/buaatrans2023:6.0.0</t>
+          <t>docker.io/zsn123/zsn20230531:0.0.1</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>93.42440000000001</v>
+        <v>94.6135</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>s_20230531190430_20230417021453</t>
+          <t>s_20230531173034_20230323102228</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -541,21 +541,21 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>77.23820000000001</v>
+        <v>66.4757</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>s_20230601103948_20230316121333</t>
+          <t>s_20230601103907_20230316121333</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>88.56854</v>
+        <v>86.17216000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -621,28 +621,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>韩毅</t>
+          <t>王章宇</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>前行者</t>
+          <t>BUAATRANS2023</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1512cc/ycc2h0ihqnu4ywa71wic:0.0.1</t>
+          <t>1982777/buaatrans2023:6.0.0</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>91.8702</v>
+        <v>93.42440000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>s_20230531225053_20230326103519</t>
+          <t>s_20230531190430_20230417021453</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -651,21 +651,21 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>77.1876</v>
+        <v>77.23820000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>s_20230603185712_20230316121333</t>
+          <t>s_20230601103948_20230316121333</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>87.46541999999999</v>
+        <v>88.56854</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -731,28 +731,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>庄伟超</t>
+          <t>韩毅</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>异乡人</t>
+          <t>前行者</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>docker.io/zsn123/zsn20230531:0.0.1</t>
+          <t>1512cc/ycc2h0ihqnu4ywa71wic:0.0.1</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>94.6135</v>
+        <v>91.8702</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>s_20230531173034_20230323102228</t>
+          <t>s_20230531225053_20230326103519</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -761,21 +761,21 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>66.4757</v>
+        <v>77.1876</v>
       </c>
       <c r="J6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>s_20230601103907_20230316121333</t>
+          <t>s_20230603185712_20230316121333</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>86.17216000000001</v>
+        <v>87.46541999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -786,28 +786,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>许庆</t>
+          <t>赵靖</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CeroChen</t>
+          <t>CodeNoob</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>chency2023/ccy_planner:0.0.3</t>
+          <t>lindgezou/leilehuimieba:0.0.1</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>90.3707</v>
+        <v>91.4478</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>s_20230531214335_20230425101926</t>
+          <t>s_20230531234345_20230326024420</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -816,21 +816,21 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>67.7586</v>
+        <v>58.487</v>
       </c>
       <c r="J7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>s_20230603185720_20230316121333</t>
+          <t>s_20230601103933_20230316121333</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>83.58707</v>
+        <v>81.55955999999999</v>
       </c>
       <c r="M7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -841,28 +841,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>赵靖</t>
+          <t>许庆</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CodeNoob</t>
+          <t>CeroChen</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>lindgezou/leilehuimieba:0.0.1</t>
+          <t>chency2023/ccy_planner:0.0.3</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>91.4478</v>
+        <v>90.3707</v>
       </c>
       <c r="F8" t="n">
         <v>7</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>s_20230531234345_20230326024420</t>
+          <t>s_20230531214335_20230425101926</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -871,21 +871,21 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>58.487</v>
+        <v>67.7586</v>
       </c>
       <c r="J8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>s_20230601103933_20230316121333</t>
+          <t>s_20230603185720_20230316121333</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>81.55955999999999</v>
+        <v>83.58707</v>
       </c>
       <c r="M8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -896,28 +896,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>庄伟超</t>
+          <t>李深</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>异乡人</t>
+          <t>Yang Liu</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>docker.io/zsn123/zsn20230602jiaochakousai:0.0.1</t>
+          <t>yangliu123123/sfhewfgjh9g43h4sv93final18:0.0.1</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>92.93689999999999</v>
+        <v>90.255</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>s_20230531235959_20230323102228</t>
+          <t>s_20230531235411_20230425082036</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -926,18 +926,18 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>53.5987</v>
+        <v>57.7411</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>s_20230603185702_20230316121333</t>
+          <t>s_20230601103941_20230316121333</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>81.13543999999999</v>
+        <v>80.50082999999999</v>
       </c>
       <c r="M9" t="n">
         <v>8</v>
@@ -951,51 +951,51 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>李深</t>
+          <t>吕超</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yang Liu</t>
+          <t>why</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>yangliu123123/sfhewfgjh9g43h4sv93final18:0.0.1</t>
+          <t>bitjacklin/ivrc666-may:0.2.0</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>90.255</v>
+        <v>85.2251</v>
       </c>
       <c r="F10" t="n">
         <v>9</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>s_20230531235411_20230425082036</t>
+          <t>s_20230531233856_20230430044055</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>CONTAINER ERROR</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>57.7411</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>s_20230601103941_20230316121333</t>
+          <t>s_20230603185728_20230316121333</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>80.50082999999999</v>
+        <v>59.65756999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -1023,7 +1023,7 @@
         <v>77.9461</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         <v>53.5896</v>
       </c>
       <c r="J11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
         <v>70.63915</v>
       </c>
       <c r="M11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -1061,48 +1061,48 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>吕超</t>
+          <t>金辉</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>why</t>
+          <t>FTJL_Soochow</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>bitjacklin/ivrc666-may:0.2.0</t>
+          <t>tangwu1122/submit-image:1.0.0</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>85.2251</v>
+        <v>61.132</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>s_20230531233856_20230430044055</t>
+          <t>s_20230531200944_20230427102135</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>CONTAINER ERROR</t>
+          <t>SUCCESS</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>54.8296</v>
       </c>
       <c r="J12" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>s_20230603185728_20230316121333</t>
+          <t>s_20230603185904_20230316121333</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>59.65756999999999</v>
+        <v>59.24127999999999</v>
       </c>
       <c r="M12" t="n">
         <v>11</v>
@@ -1116,28 +1116,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>金辉</t>
+          <t>李绍松</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>FTJL_Soochow</t>
+          <t>张同学</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>tangwu1122/submit-image:1.0.0</t>
+          <t>mark857/test-image-for-1656:0.0.3</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>61.132</v>
+        <v>58.152</v>
       </c>
       <c r="F13" t="n">
         <v>12</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>s_20230531200944_20230427102135</t>
+          <t>s_20230529163025_20230426075406</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1146,18 +1146,18 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>54.8296</v>
+        <v>52.3064</v>
       </c>
       <c r="J13" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>s_20230603185904_20230316121333</t>
+          <t>s_20230604114056_20230316121333</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>59.24127999999999</v>
+        <v>56.39831999999999</v>
       </c>
       <c r="M13" t="n">
         <v>12</v>
@@ -1171,28 +1171,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>李绍松</t>
+          <t>田野</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>张同学</t>
+          <t>liuyiru</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>mark857/test-image-for-1656:0.0.3</t>
+          <t>yiruliu/test-image-for-onsite:1.1.3</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>58.152</v>
+        <v>52.1444</v>
       </c>
       <c r="F14" t="n">
         <v>13</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>s_20230529163025_20230426075406</t>
+          <t>s_20230410105329_20230307041118</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1201,18 +1201,18 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>52.3064</v>
+        <v>46.4433</v>
       </c>
       <c r="J14" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>s_20230604114056_20230316121333</t>
+          <t>s_20230604114107_20230316121333</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>56.39831999999999</v>
+        <v>50.43406999999999</v>
       </c>
       <c r="M14" t="n">
         <v>13</v>
@@ -1226,28 +1226,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>田野</t>
+          <t>王润民</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>liuyiru</t>
+          <t>trytest</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>yiruliu/test-image-for-onsite:1.1.3</t>
+          <t>5945docker/onsite-chd-trytest:0.0.1</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>52.1444</v>
+        <v>48.8162</v>
       </c>
       <c r="F15" t="n">
         <v>14</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>s_20230410105329_20230307041118</t>
+          <t>s_20230514123219_20230319091600</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1256,18 +1256,18 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>46.4433</v>
+        <v>50.0576</v>
       </c>
       <c r="J15" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>s_20230604114107_20230316121333</t>
+          <t>s_20230604114117_20230316121333</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>50.43406999999999</v>
+        <v>49.18862</v>
       </c>
       <c r="M15" t="n">
         <v>14</v>
@@ -1281,28 +1281,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>王润民</t>
+          <t>赵栓峰</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>trytest</t>
+          <t>乐平举世无双</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5945docker/onsite-chd-trytest:0.0.1</t>
+          <t>15207304095/test-onsite:0.0.6</t>
         </is>
       </c>
       <c r="E16" t="n">
         <v>48.8162</v>
       </c>
       <c r="F16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>s_20230514123219_20230319091600</t>
+          <t>s_20230425221834_20230419040432</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1314,18 +1314,18 @@
         <v>50.0576</v>
       </c>
       <c r="J16" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>s_20230604114117_20230316121333</t>
+          <t>s_20230604114131_20230316121333</t>
         </is>
       </c>
       <c r="L16" t="n">
         <v>49.18862</v>
       </c>
       <c r="M16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1336,106 +1336,51 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>赵栓峰</t>
+          <t>黄玮</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>乐平举世无双</t>
+          <t>ycycycl</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15207304095/test-onsite:0.0.6</t>
+          <t>kunxuchen/take-to-use-to-test:0.1.1</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>48.8162</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
+        <v>16</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>s_20230524110939_20230430113500</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
         <v>15</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>s_20230425221834_20230419040432</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>50.0576</v>
-      </c>
-      <c r="J17" t="n">
-        <v>13</v>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>s_20230604114131_20230316121333</t>
+          <t>s_20230604114044_20230316121333</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>49.18862</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>第一届OnSite自动驾驶算法挑战赛（交叉口专项赛）</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>黄玮</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>ycycycl</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>kunxuchen/take-to-use-to-test:0.1.1</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>17</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>s_20230524110939_20230430113500</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
         <v>16</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>s_20230604114044_20230316121333</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1449,7 +1394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1587,48 +1532,48 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>许庆</t>
+          <t>庄伟超</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CeroChen</t>
+          <t>FF_T</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>chency2023/zzh_planner:0.0.3</t>
+          <t>docker.io/tffff/0526version:0.0.1</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>91.5508</v>
+        <v>92.6397</v>
       </c>
       <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>s_20230530203925_20230323100625</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>68.3432</v>
+      </c>
+      <c r="J3" t="n">
         <v>4</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>s_20230531220417_20230425101926</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>69.6314</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3</v>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>s_20230601103306_20230316121333</t>
+          <t>s_20230604204114_20230316121333</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>84.97497999999999</v>
+        <v>85.35075000000001</v>
       </c>
       <c r="M3" t="n">
         <v>2</v>
@@ -1642,51 +1587,51 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>秦晓辉</t>
+          <t>李深</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>binjie</t>
+          <t>Yang Liu</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lylez/cnfe-morning-night:0.5.4</t>
+          <t>yangliu123123/skhfgiewbw2i4ht982bf2final20:0.0.1</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>90.83329999999999</v>
+        <v>91.9783</v>
       </c>
       <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>s_20230531235959_20230425082036</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>66.68089999999999</v>
+      </c>
+      <c r="J4" t="n">
         <v>5</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>s_20230531104349_20230411085828</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>70.2403</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>s_20230601103300_20230316121333</t>
+          <t>s_20230606112942_20230316121333</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>84.65539999999999</v>
+        <v>84.38908000000001</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -1697,28 +1642,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>庄伟超</t>
+          <t>许庆</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>异乡人</t>
+          <t>CeroChen</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>docker.io/zsn123/zsn20230602zonghesai:0.0.1</t>
+          <t>chency2023/zzh_planner:0.0.3</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>81.497</v>
+        <v>91.5508</v>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>s_20230531235958_20230323102228</t>
+          <t>s_20230531220417_20230425101926</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -1727,21 +1672,21 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>59.187</v>
+        <v>69.6314</v>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>s_20230603190030_20230316121333</t>
+          <t>s_20230601103306_20230316121333</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>74.804</v>
+        <v>84.97497999999999</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1752,28 +1697,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>裴晓飞</t>
+          <t>秦晓辉</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>huzhilong</t>
+          <t>binjie</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>huzhilong/end:1.5</t>
+          <t>lylez/cnfe-morning-night:0.5.4</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>79.3091</v>
+        <v>90.83329999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>s_20230531172908_20230318012446</t>
+          <t>s_20230531104349_20230411085828</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1782,21 +1727,21 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>57.983</v>
+        <v>70.2403</v>
       </c>
       <c r="J6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>s_20230601103334_20230316121333</t>
+          <t>s_20230601103300_20230316121333</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>72.91127</v>
+        <v>84.65539999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1807,48 +1752,48 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>庄伟超</t>
+          <t>裴晓飞</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FF_T</t>
+          <t>huzhilong</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>docker.io/tffff/0526version:0.0.1</t>
+          <t>huzhilong/end:1.5</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>92.6397</v>
+        <v>79.3091</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>s_20230530203925_20230323100625</t>
+          <t>s_20230531172908_20230318012446</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>EVALUATE ERROR</t>
+          <t>SUCCESS</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>57.983</v>
       </c>
       <c r="J7" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>s_20230528165857_20230316121333</t>
+          <t>s_20230601103334_20230316121333</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>64.84779</v>
+        <v>72.91127</v>
       </c>
       <c r="M7" t="n">
         <v>6</v>
@@ -1879,7 +1824,7 @@
         <v>67.40600000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1895,7 +1840,7 @@
         <v>53.6496</v>
       </c>
       <c r="J8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -1917,51 +1862,51 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>单肖年</t>
+          <t>赵克刚</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>yzbyx</t>
+          <t>HZW</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>yzbyx/atjhyt7txlebsfbcmzh:1.0.1</t>
+          <t>jaminhong/sougoukonn:1.1</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>65.1097</v>
+        <v>65.99630000000001</v>
       </c>
       <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>s_20230530181009_20230321054337</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>43.2928</v>
+      </c>
+      <c r="J9" t="n">
         <v>10</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>s_20230531235959_20230430094609</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>53.3885</v>
-      </c>
-      <c r="J9" t="n">
-        <v>7</v>
-      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>s_20230604120107_20230316121333</t>
+          <t>s_20230603190052_20230316121333</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>61.59334</v>
+        <v>59.18525</v>
       </c>
       <c r="M9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -1972,28 +1917,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>赵克刚</t>
+          <t>单肖年</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HZW</t>
+          <t>yzbyx</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>jaminhong/sougoukonn:1.1</t>
+          <t>yzbyx/atjhyt7txlebsfbcmzh:1.0.1</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>65.99630000000001</v>
+        <v>65.1097</v>
       </c>
       <c r="F10" t="n">
         <v>9</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>s_20230530181009_20230321054337</t>
+          <t>s_20230531235959_20230430094609</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -2002,21 +1947,21 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>43.2928</v>
+        <v>53.3885</v>
       </c>
       <c r="J10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>s_20230603190052_20230316121333</t>
+          <t>s_20230604120107_20230316121333</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>59.18525</v>
+        <v>61.59334</v>
       </c>
       <c r="M10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -2044,7 +1989,7 @@
         <v>58.6781</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2060,7 +2005,7 @@
         <v>52.9085</v>
       </c>
       <c r="J11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -2073,53 +2018,6 @@
       <c r="M11" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>第一届OnSite自动驾驶算法挑战赛（综合赛）</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>李深</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Yang Liu</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>yangliu123123/sfhewfgjh9g43h4sv93final18:0.0.1</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>92.06399999999999</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>s_20230531235351_20230425082036</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>TESTING</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>s_20230601103327_20230316121333</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2270,51 +2168,51 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>曲栩</t>
+          <t>冉斌</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>skroop</t>
+          <t>HaotianShi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>anbc/hnfzpuwbf6r3gxwea9gw:v13</t>
+          <t>breakice/hlfw2023:0.0.6</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>93.03579999999999</v>
+        <v>93.0772</v>
       </c>
       <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>s_20230531234852_20230427114805</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>91.2927</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>s_20230601104109_20230316121333</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>92.54185</v>
+      </c>
+      <c r="M3" t="n">
         <v>3</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>s_20230530162858_20230409034310</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>92.2867</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>s_20230601104053_20230316121333</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>92.81106999999999</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -2325,51 +2223,51 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>冉斌</t>
+          <t>曲栩</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HaotianShi</t>
+          <t>skroop</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>breakice/hlfw2023:0.0.6</t>
+          <t>anbc/hnfzpuwbf6r3gxwea9gw:v13</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>93.0772</v>
+        <v>93.03579999999999</v>
       </c>
       <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>s_20230530162858_20230409034310</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>92.2867</v>
+      </c>
+      <c r="J4" t="n">
         <v>2</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>s_20230531234852_20230427114805</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>91.2927</v>
-      </c>
-      <c r="J4" t="n">
-        <v>7</v>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>s_20230601104109_20230316121333</t>
+          <t>s_20230601104053_20230316121333</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>92.54185</v>
+        <v>92.81106999999999</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -3205,28 +3103,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>陈志成</t>
+          <t>杨澜</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>13992122688</t>
+          <t>小fu同xuo</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>xxf6/jiasheng27-test-image-for-onsite:0.0.1</t>
+          <t>shigezhi/finalfreeway6f829gf8ywsd890fb928f23f18:0.0.9</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>71.0286</v>
+        <v>76.6421</v>
       </c>
       <c r="F20" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>s_20230527160218_20230424101455</t>
+          <t>s_20230530222724_20230322113454</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -3235,21 +3133,21 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>69.953</v>
+        <v>29.5674</v>
       </c>
       <c r="J20" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>s_20230604113456_20230316121333</t>
+          <t>s_20230604114014_20230316121333</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>70.70591999999999</v>
+        <v>62.51969</v>
       </c>
       <c r="M20" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -3260,28 +3158,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>王润民</t>
+          <t>陈志成</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>trytest</t>
+          <t>13992122688</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5945docker/onsite-highway-chd-hmc-trytest:0.0.1</t>
+          <t>xxf6/jiasheng27-test-image-for-onsite:0.0.1</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>68.7261</v>
+        <v>71.0286</v>
       </c>
       <c r="F21" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>s_20230514204435_20230319091600</t>
+          <t>s_20230527160218_20230424101455</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -3290,21 +3188,21 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>68.6448</v>
+        <v>69.953</v>
       </c>
       <c r="J21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>s_20230604113924_20230316121333</t>
+          <t>s_20230604113456_20230316121333</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>68.70170999999999</v>
+        <v>70.70591999999999</v>
       </c>
       <c r="M21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -3315,28 +3213,28 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>闵海根</t>
+          <t>王润民</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>yyb</t>
+          <t>trytest</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ppdxqn/test-image-for-onsite:0.0.2</t>
+          <t>5945docker/onsite-highway-chd-hmc-trytest:0.0.1</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>68.4966</v>
+        <v>68.7261</v>
       </c>
       <c r="F22" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>s_20230505154752_20230425110902</t>
+          <t>s_20230514204435_20230319091600</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -3352,14 +3250,14 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>s_20230604113712_20230316121333</t>
+          <t>s_20230604113924_20230316121333</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>68.54106</v>
+        <v>68.70170999999999</v>
       </c>
       <c r="M22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -3370,28 +3268,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>杨澜</t>
+          <t>闵海根</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>小fu同xuo</t>
+          <t>yyb</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>shigezhi/finalfreeway6f829gf8ywsd890fb928f23f18:0.0.9</t>
+          <t>ppdxqn/test-image-for-onsite:0.0.2</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>76.6421</v>
+        <v>68.4966</v>
       </c>
       <c r="F23" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>s_20230530222724_20230322113454</t>
+          <t>s_20230505154752_20230425110902</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -3400,21 +3298,21 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>29.6874</v>
+        <v>68.6448</v>
       </c>
       <c r="J23" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>s_20230531094644_20230316121333</t>
+          <t>s_20230604113712_20230316121333</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>62.55568999999999</v>
+        <v>68.54106</v>
       </c>
       <c r="M23" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
@@ -3510,18 +3408,18 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>60.0321</v>
+        <v>59.8821</v>
       </c>
       <c r="J25" t="n">
         <v>23</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>s_20230531095038_20230316121333</t>
+          <t>s_20230604113526_20230316121333</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>58.32675999999999</v>
+        <v>58.28176</v>
       </c>
       <c r="M25" t="n">
         <v>24</v>
@@ -3676,51 +3574,51 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>马峻岩</t>
+          <t>李道飞</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>liboxuan2457</t>
+          <t>CLH ZJU</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>liboxuan/lbxhtzwjlyhggxhrhc:0.0.4</t>
+          <t>sennawhite/btiuxldbterqeolrdfimnfqugdduznawexhgqmezjonymdxzchyzvrbbbnhgwczyfkcfrreuzwvzeumzzcgacymqasttptuhbqur:0.11.1</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>96.1041</v>
+        <v>96.4773</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>s_20230531051225_20230430104525</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>66.5552</v>
+      </c>
+      <c r="J2" t="n">
         <v>2</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>s_20230531223434_20230319065149</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>68.5741</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>s_20230603185246_20230316121333</t>
+          <t>s_20230603185237_20230316121333</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>87.8451</v>
+        <v>87.50067</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -3731,51 +3629,51 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>李道飞</t>
+          <t>马峻岩</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CLH ZJU</t>
+          <t>liboxuan2457</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sennawhite/btiuxldbterqeolrdfimnfqugdduznawexhgqmezjonymdxzchyzvrbbbnhgwczyfkcfrreuzwvzeumzzcgacymqasttptuhbqur:0.11.1</t>
+          <t>liboxuan/lbxhtzwjlyhggxhrhc:0.0.4</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>96.4773</v>
+        <v>96.1041</v>
       </c>
       <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>s_20230531223434_20230319065149</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>68.5741</v>
+      </c>
+      <c r="J3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>s_20230531051225_20230430104525</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>66.5552</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>s_20230603185237_20230316121333</t>
+          <t>s_20230603185246_20230316121333</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>87.50067</v>
+        <v>87.8451</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -3786,28 +3684,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>韩毅</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>前行者</t>
-        </is>
+          <t>韩嘉懿</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>17368760800</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1512cc/24koqsxodgxff9pt64dn:0.0.1</t>
+          <t>xxf6/merge61-test-image-for-onsite:0.0.1</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>94.6065</v>
+        <v>95.85290000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>s_20230531195621_20230326103519</t>
+          <t>s_20230531235959_ 20230418111048</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -3816,21 +3712,21 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>64.8561</v>
+        <v>61.771</v>
       </c>
       <c r="J4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>s_20230603185319_20230316121333</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>85.62833000000001</v>
+      </c>
+      <c r="M4" t="n">
         <v>4</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>s_20230601103800_20230316121333</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>85.68137999999999</v>
-      </c>
-      <c r="M4" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -3841,26 +3737,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>韩嘉懿</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>17368760800</v>
+          <t>贺宜</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ITS_Panda</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>xxf6/merge61-test-image-for-onsite:0.0.1</t>
+          <t>sssusheng/effigy-trophy-gypsy-thumq:0.0.7</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>95.85290000000001</v>
+        <v>95.1204</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>s_20230531235959_ 20230418111048</t>
+          <t>s_20230531090544_20230402035710</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -3869,21 +3767,21 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>61.771</v>
+        <v>63.356</v>
       </c>
       <c r="J5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>s_20230603185319_20230316121333</t>
+          <t>s_20230604120520_20230316121333</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>85.62833000000001</v>
+        <v>85.59107999999999</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -3894,51 +3792,51 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>贺宜</t>
+          <t>韩毅</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ITS_Panda</t>
+          <t>前行者</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sssusheng/effigy-trophy-gypsy-thumq:0.0.7</t>
+          <t>1512cc/24koqsxodgxff9pt64dn:0.0.1</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>95.1204</v>
+        <v>94.6065</v>
       </c>
       <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>s_20230531195621_20230326103519</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>64.8561</v>
+      </c>
+      <c r="J6" t="n">
         <v>4</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>s_20230531090544_20230402035710</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>63.356</v>
-      </c>
-      <c r="J6" t="n">
-        <v>5</v>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>s_20230604120520_20230316121333</t>
+          <t>s_20230601103800_20230316121333</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>85.59107999999999</v>
+        <v>85.68137999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -3949,51 +3847,51 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>闵海根</t>
+          <t>刘丛志</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>yyb</t>
+          <t>WenxuanXiao</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>studentxia/xiaoxia:0.0.16</t>
+          <t>xiaowenxaun/image_from_cqu:0.0.7</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>91.7334</v>
+        <v>94.5204</v>
       </c>
       <c r="F7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>s_20230531235945_20230424092505</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>51.0088</v>
+      </c>
+      <c r="J7" t="n">
+        <v>9</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>s_20230601103734_20230316121333</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>81.46691999999999</v>
+      </c>
+      <c r="M7" t="n">
         <v>7</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>s_20230531233655_20230425110902</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>66.3946</v>
-      </c>
-      <c r="J7" t="n">
-        <v>3</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>s_20230604113202_20230316121333</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>84.13176</v>
-      </c>
-      <c r="M7" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -4004,51 +3902,51 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>刘丛志</t>
+          <t>闵海根</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>WenxuanXiao</t>
+          <t>yyb</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xiaowenxaun/image_from_cqu:0.0.7</t>
+          <t>studentxia/xiaoxia:0.0.16</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>94.5204</v>
+        <v>91.7334</v>
       </c>
       <c r="F8" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>s_20230531233655_20230425110902</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>66.3946</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>s_20230604113202_20230316121333</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>84.13176</v>
+      </c>
+      <c r="M8" t="n">
         <v>6</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>s_20230531235945_20230424092505</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>51.0088</v>
-      </c>
-      <c r="J8" t="n">
-        <v>9</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>s_20230601103734_20230316121333</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>81.46691999999999</v>
-      </c>
-      <c r="M8" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -4096,7 +3994,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>s_20230527231958_20230316121333</t>
+          <t>s_20230603185353_20230316121333</t>
         </is>
       </c>
       <c r="L9" t="n">
@@ -4151,7 +4049,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>s_20230531091423_20230316121333</t>
+          <t>s_20230603185358_20230316121333</t>
         </is>
       </c>
       <c r="L10" t="n">

</xml_diff>